<commit_message>
Fixed the bug where you could only edit the Excel database while it was open
</commit_message>
<xml_diff>
--- a/VMat/VMat/VirtualList.xlsx
+++ b/VMat/VMat/VirtualList.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="TestSheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet sheetId="1" r:id="rId1" name="TestSheet"/>
+    <sheet sheetId="2" r:id="rId2" name="Sheet2"/>
+    <sheet sheetId="3" r:id="rId3" name="Sheet3"/>
   </sheets>
   <definedNames>
-    <definedName name="TestName">TestSheet!$A$1:$B$3</definedName>
+    <definedName name="TestName">TestSheet!$A$1:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -374,16 +374,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row spans="1:2" outlineLevel="0" r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,20 +391,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
+    <row spans="1:2" outlineLevel="0" r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Jacob</t>
+        </is>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row spans="1:2" outlineLevel="0" r="3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>Eleanor</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Rigsby</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>